<commit_message>
admin and profile update
</commit_message>
<xml_diff>
--- a/mernbackend/src/upload/order.xlsx
+++ b/mernbackend/src/upload/order.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,7 +430,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>6444a94280ca9ea5d90965f0</v>
+        <v>6444a94ddcf231be420f538f</v>
       </c>
       <c r="B2" t="str">
         <v>audi</v>
@@ -456,25 +456,25 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>6444a94ddcf231be420f538f</v>
+        <v>6444c93c4a460f434caed613</v>
       </c>
       <c r="B3" t="str">
         <v>audi</v>
       </c>
       <c r="C3" t="str">
-        <v>london</v>
+        <v>katargam</v>
       </c>
       <c r="D3" t="str">
-        <v>prince homes</v>
+        <v>varacha</v>
       </c>
       <c r="E3" t="str">
         <v>2023-04-12</v>
       </c>
       <c r="F3" t="str">
-        <v>2023-04-24</v>
+        <v>2023-04-26</v>
       </c>
       <c r="G3" t="str">
-        <v>42900.00</v>
+        <v>49500.00</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>6444c93c4a460f434caed613</v>
+        <v>6444c94f76dc7da282a7a556</v>
       </c>
       <c r="B4" t="str">
         <v>audi</v>
@@ -508,25 +508,25 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>6444c94f76dc7da282a7a556</v>
+        <v>6444ca167b73ab12b739b122</v>
       </c>
       <c r="B5" t="str">
         <v>audi</v>
       </c>
       <c r="C5" t="str">
-        <v>katargam</v>
+        <v>london</v>
       </c>
       <c r="D5" t="str">
-        <v>varacha</v>
+        <v xml:space="preserve">mansi </v>
       </c>
       <c r="E5" t="str">
-        <v>2023-04-12</v>
+        <v>2023-04-10</v>
       </c>
       <c r="F5" t="str">
-        <v>2023-04-26</v>
+        <v>2023-04-19</v>
       </c>
       <c r="G5" t="str">
-        <v>49500.00</v>
+        <v>33000.00</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -534,25 +534,25 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>6444ca167b73ab12b739b122</v>
+        <v>6444ca377b73ab12b739b12e</v>
       </c>
       <c r="B6" t="str">
-        <v>audi</v>
+        <v>Mercedes</v>
       </c>
       <c r="C6" t="str">
-        <v>london</v>
+        <v>katargam</v>
       </c>
       <c r="D6" t="str">
-        <v xml:space="preserve">mansi </v>
+        <v>prince homes</v>
       </c>
       <c r="E6" t="str">
-        <v>2023-04-10</v>
+        <v>2023-04-17</v>
       </c>
       <c r="F6" t="str">
-        <v>2023-04-19</v>
+        <v>2023-04-26</v>
       </c>
       <c r="G6" t="str">
-        <v>33000.00</v>
+        <v>22000.00</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -560,33 +560,85 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>6444ca377b73ab12b739b12e</v>
+        <v>6444eefa0181a0655cdd09bd</v>
       </c>
       <c r="B7" t="str">
-        <v>Mercedes</v>
+        <v>audi</v>
       </c>
       <c r="C7" t="str">
-        <v>katargam</v>
+        <v>america</v>
       </c>
       <c r="D7" t="str">
-        <v>prince homes</v>
+        <v>mumbai</v>
       </c>
       <c r="E7" t="str">
+        <v>2023-04-20</v>
+      </c>
+      <c r="F7" t="str">
+        <v>2023-04-27</v>
+      </c>
+      <c r="G7" t="str">
+        <v>26400.00</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>6444ef7c0181a0655cdd09db</v>
+      </c>
+      <c r="B8" t="str">
+        <v xml:space="preserve">Toyota Innova </v>
+      </c>
+      <c r="C8" t="str">
+        <v>rajkot</v>
+      </c>
+      <c r="D8" t="str">
+        <v>mumbai</v>
+      </c>
+      <c r="E8" t="str">
+        <v>2023-04-14</v>
+      </c>
+      <c r="F8" t="str">
+        <v>2023-04-28</v>
+      </c>
+      <c r="G8" t="str">
+        <v>33000.00</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>644663592cb7d38a677d1201</v>
+      </c>
+      <c r="B9" t="str">
+        <v>mini cooper</v>
+      </c>
+      <c r="C9" t="str">
+        <v>surat</v>
+      </c>
+      <c r="D9" t="str">
+        <v xml:space="preserve">mansi </v>
+      </c>
+      <c r="E9" t="str">
         <v>2023-04-17</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F9" t="str">
         <v>2023-04-26</v>
       </c>
-      <c r="G7" t="str">
-        <v>22000.00</v>
-      </c>
-      <c r="H7">
+      <c r="G9" t="str">
+        <v>55000.00</v>
+      </c>
+      <c r="H9">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>